<commit_message>
Backup up to Advance JS
</commit_message>
<xml_diff>
--- a/GUI Basic Learning/GUI basic Training.xlsx
+++ b/GUI Basic Learning/GUI basic Training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhruvil Dobariya - 335\GUI Basic Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C827F01-DF65-40C6-9A13-A6C84B09CA54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3AA803-E4CA-4327-A188-CB5D3AE895A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Topic</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Actual Time</t>
+  </si>
+  <si>
+    <t>Basic of jQuery</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,6 +580,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -895,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1510,9 +1516,13 @@
     </row>
     <row r="52" spans="1:7" ht="15.75">
       <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
+      <c r="B52" s="11">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="D52" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
@@ -1529,6 +1539,9 @@
       <c r="F53">
         <v>0.5</v>
       </c>
+      <c r="G53" s="18">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="31.5">
       <c r="A54" s="9"/>
@@ -1543,6 +1556,9 @@
       <c r="F54">
         <v>0.5</v>
       </c>
+      <c r="G54" s="18">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="15.75">
       <c r="A55" s="9"/>
@@ -1559,6 +1575,9 @@
       <c r="F55">
         <v>4</v>
       </c>
+      <c r="G55" s="18">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="15.75">
       <c r="A56" s="9"/>
@@ -1575,6 +1594,9 @@
       <c r="F56">
         <v>8</v>
       </c>
+      <c r="G56" s="18">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="15.75">
       <c r="A57" s="3"/>
@@ -1602,6 +1624,9 @@
       <c r="F58" s="19">
         <v>10</v>
       </c>
+      <c r="G58" s="20">
+        <v>10.25</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="15.75">
       <c r="A59" s="9"/>
@@ -1614,6 +1639,7 @@
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="19"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" spans="1:7" ht="15.75">
       <c r="A60" s="9"/>
@@ -1626,6 +1652,7 @@
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="19"/>
+      <c r="G60" s="20"/>
     </row>
     <row r="61" spans="1:7" ht="15.75">
       <c r="A61" s="3"/>
@@ -1648,6 +1675,12 @@
         <v>107</v>
       </c>
       <c r="E62" s="10"/>
+      <c r="F62">
+        <v>4</v>
+      </c>
+      <c r="G62" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="63" spans="1:7" ht="15.75">
       <c r="A63" s="9"/>
@@ -1659,6 +1692,12 @@
         <v>109</v>
       </c>
       <c r="E63" s="10"/>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63" s="18">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="15.75">
       <c r="A64" s="3"/>
@@ -1672,8 +1711,14 @@
       <c r="E64" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75">
+      <c r="F64">
+        <v>8</v>
+      </c>
+      <c r="G64" s="18">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75">
       <c r="A65" s="3"/>
       <c r="B65" s="11">
         <v>5.5</v>
@@ -1683,8 +1728,14 @@
         <v>112</v>
       </c>
       <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="1:5" ht="15.75">
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75">
       <c r="A66" s="3"/>
       <c r="B66" s="11">
         <v>5.6</v>
@@ -1696,8 +1747,14 @@
       <c r="E66" s="13" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75">
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75">
       <c r="A67" s="12"/>
       <c r="B67" s="11">
         <v>5.7</v>
@@ -1710,7 +1767,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75">
+    <row r="68" spans="1:7" ht="15.75">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="14" t="s">
@@ -1720,8 +1777,14 @@
         <v>118</v>
       </c>
       <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75">
+      <c r="F68">
+        <v>0.5</v>
+      </c>
+      <c r="G68" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="14" t="s">
@@ -1731,8 +1794,14 @@
         <v>120</v>
       </c>
       <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75">
+      <c r="F69">
+        <v>0.5</v>
+      </c>
+      <c r="G69" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="14" t="s">
@@ -1742,8 +1811,14 @@
         <v>122</v>
       </c>
       <c r="E70" s="10"/>
-    </row>
-    <row r="71" spans="1:5" ht="31.5">
+      <c r="F70">
+        <v>4</v>
+      </c>
+      <c r="G70" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="31.5">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="14" t="s">
@@ -1753,8 +1828,14 @@
         <v>124</v>
       </c>
       <c r="E71" s="10"/>
-    </row>
-    <row r="72" spans="1:5" ht="15.75">
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="14" t="s">
@@ -1766,8 +1847,14 @@
       <c r="E72" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75">
+      <c r="F72">
+        <v>0.5</v>
+      </c>
+      <c r="G72" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="14" t="s">
@@ -1777,15 +1864,21 @@
         <v>129</v>
       </c>
       <c r="E73" s="14"/>
-    </row>
-    <row r="74" spans="1:5" ht="15.75">
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="14"/>
       <c r="D74" s="10"/>
       <c r="E74" s="14"/>
     </row>
-    <row r="75" spans="1:5" ht="37.5">
+    <row r="75" spans="1:7" ht="37.5">
       <c r="A75" s="5">
         <v>6</v>
       </c>
@@ -1795,10 +1888,14 @@
         <v>130</v>
       </c>
       <c r="E75" s="7"/>
+      <c r="F75">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F58:F60"/>
+    <mergeCell ref="G58:G60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{EDDDB51D-1748-4951-8AD4-4A732F687A86}"/>
@@ -1818,16 +1915,11 @@
     <hyperlink ref="E66" r:id="rId15" xr:uid="{CE3147EC-08D4-4841-AED4-2C0E4A5A186F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012D490038F304647A208A56C93ACD3FB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="52551bb2fc9acff2d7c3d8f36be04736">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="85df923e-d879-42f4-9cd5-d99571c2edb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f80b649ded2497a6e2fb6f2f393f013" ns2:_="">
     <xsd:import namespace="85df923e-d879-42f4-9cd5-d99571c2edb5"/>
@@ -1959,7 +2051,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1968,23 +2060,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{100FB3B0-611D-4E68-B442-F0B4A7055530}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="85df923e-d879-42f4-9cd5-d99571c2edb5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{627D361D-E639-436C-B595-292307492D8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2002,10 +2084,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D008A29A-16EE-48F2-A304-97B47DA205E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{100FB3B0-611D-4E68-B442-F0B4A7055530}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="85df923e-d879-42f4-9cd5-d99571c2edb5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>